<commit_message>
fixed issue when it didn't work on 1 processor
</commit_message>
<xml_diff>
--- a/Analytics.xlsx
+++ b/Analytics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12180" windowWidth="19200" windowHeight="11820" tabRatio="500"/>
+    <workbookView xWindow="19200" yWindow="440" windowWidth="19200" windowHeight="23460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -56,13 +56,13 @@
     <t>tTime</t>
   </si>
   <si>
-    <t>64x64</t>
-  </si>
-  <si>
     <t>16x16</t>
   </si>
   <si>
     <t>1024x1024</t>
+  </si>
+  <si>
+    <t>256x256</t>
   </si>
 </sst>
 </file>
@@ -318,10 +318,10 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.201082006127688</c:v>
+                  <c:v>0.309985165955869</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0398039579941209</c:v>
+                  <c:v>0.146876647337902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,10 +407,10 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.599158321558027</c:v>
+                  <c:v>0.568338624648977</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.228921177409511</c:v>
+                  <c:v>0.255715445062449</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -495,10 +495,10 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.764993123919032</c:v>
+                  <c:v>1.384346349876535</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.367303953970286</c:v>
+                  <c:v>0.983526939944379</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -513,11 +513,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1986667008"/>
-        <c:axId val="-1987691040"/>
+        <c:axId val="-1755970208"/>
+        <c:axId val="-1755962608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1986667008"/>
+        <c:axId val="-1755970208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,7 +563,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -593,6 +592,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -629,12 +629,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1987691040"/>
+        <c:crossAx val="-1755962608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1987691040"/>
+        <c:axId val="-1755962608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,7 +680,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -746,7 +745,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1986667008"/>
+        <c:crossAx val="-1755970208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -760,7 +759,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -863,7 +861,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -974,13 +971,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.01457</c:v>
+                  <c:v>0.006687</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.036229</c:v>
+                  <c:v>0.010786</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.091511</c:v>
+                  <c:v>0.011382</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1062,13 +1059,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.03901</c:v>
+                  <c:v>0.155028</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.032554</c:v>
+                  <c:v>0.136387</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.042602</c:v>
+                  <c:v>0.151563</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1150,13 +1147,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.267888</c:v>
+                  <c:v>12.181229</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.443095</c:v>
+                  <c:v>4.399632</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.58551</c:v>
+                  <c:v>3.096313</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1171,11 +1168,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1986579408"/>
-        <c:axId val="-1986575648"/>
+        <c:axId val="-1755900256"/>
+        <c:axId val="-1755896864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1986579408"/>
+        <c:axId val="-1755900256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1221,7 +1218,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1287,12 +1283,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1986575648"/>
+        <c:crossAx val="-1755896864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1986575648"/>
+        <c:axId val="-1755896864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,7 +1334,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1404,7 +1399,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1986579408"/>
+        <c:crossAx val="-1755900256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1418,7 +1413,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1570,10 +1564,10 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.402164012255376</c:v>
+                  <c:v>0.619970331911737</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.159215831976484</c:v>
+                  <c:v>0.587506589351608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1658,10 +1652,10 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.198316643116053</c:v>
+                  <c:v>1.136677249297954</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.915684709638045</c:v>
+                  <c:v>1.022861780249797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1746,10 +1740,10 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.529986247838064</c:v>
+                  <c:v>2.76869269975307</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.469215815881144</c:v>
+                  <c:v>3.934107759777516</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1764,11 +1758,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1986533712"/>
-        <c:axId val="-1986529952"/>
+        <c:axId val="-1755843504"/>
+        <c:axId val="-1755840112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1986533712"/>
+        <c:axId val="-1755843504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1814,7 +1808,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1881,12 +1874,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1986529952"/>
+        <c:crossAx val="-1755840112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1986529952"/>
+        <c:axId val="-1755840112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1932,7 +1925,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1998,7 +1990,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1986533712"/>
+        <c:crossAx val="-1755843504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2012,7 +2004,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3746,7 +3737,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="139" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3768,7 +3759,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="139" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3779,7 +3770,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8678333" cy="6284872"/>
+    <xdr:ext cx="8661583" cy="6276906"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3833,7 +3824,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8678333" cy="6284872"/>
+    <xdr:ext cx="8661583" cy="6276906"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4122,7 +4113,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4159,34 +4150,34 @@
         <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>1.457E-2</v>
+        <v>6.6870000000000002E-3</v>
       </c>
       <c r="D2" s="5">
         <f>$C$2/C2</f>
         <v>1</v>
       </c>
       <c r="E2" s="5">
-        <f>D2/B2</f>
+        <f t="shared" ref="E2:E10" si="0">D2/B2</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
       </c>
       <c r="C3" s="5">
-        <v>3.6228999999999997E-2</v>
+        <v>1.0786E-2</v>
       </c>
       <c r="D3" s="5">
         <f>$C$2/C3</f>
-        <v>0.40216401225537557</v>
+        <v>0.61997033191173745</v>
       </c>
       <c r="E3" s="5">
-        <f>D3/B3</f>
-        <v>0.20108200612768778</v>
+        <f t="shared" si="0"/>
+        <v>0.30998516595586872</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="26" x14ac:dyDescent="0.3">
@@ -4195,15 +4186,15 @@
         <v>4</v>
       </c>
       <c r="C4" s="5">
-        <v>9.1510999999999995E-2</v>
+        <v>1.1382E-2</v>
       </c>
       <c r="D4" s="5">
         <f>$C$2/C4</f>
-        <v>0.1592158319764837</v>
+        <v>0.58750658935160782</v>
       </c>
       <c r="E4" s="5">
-        <f>D4/B4</f>
-        <v>3.9803957994120925E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.14687664733790196</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="26" x14ac:dyDescent="0.3">
@@ -4214,34 +4205,34 @@
         <v>1</v>
       </c>
       <c r="C5" s="9">
-        <v>3.9010000000000003E-2</v>
+        <v>0.155028</v>
       </c>
       <c r="D5" s="9">
         <f>$C$5/C5</f>
         <v>1</v>
       </c>
       <c r="E5" s="9">
-        <f>D5/B5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <v>3.2554E-2</v>
+        <v>0.13638700000000001</v>
       </c>
       <c r="D6" s="5">
         <f>$C$5/C6</f>
-        <v>1.1983166431160535</v>
+        <v>1.1366772492979536</v>
       </c>
       <c r="E6" s="5">
-        <f>D6/B6</f>
-        <v>0.59915832155802673</v>
+        <f t="shared" si="0"/>
+        <v>0.56833862464897678</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26" x14ac:dyDescent="0.3">
@@ -4250,15 +4241,15 @@
         <v>4</v>
       </c>
       <c r="C7" s="5">
-        <v>4.2602000000000001E-2</v>
+        <v>0.151563</v>
       </c>
       <c r="D7" s="5">
         <f>$C$5/C7</f>
-        <v>0.91568470963804516</v>
+        <v>1.022861780249797</v>
       </c>
       <c r="E7" s="5">
-        <f>D7/B7</f>
-        <v>0.22892117740951129</v>
+        <f t="shared" si="0"/>
+        <v>0.25571544506244925</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="26" x14ac:dyDescent="0.3">
@@ -4269,34 +4260,34 @@
         <v>1</v>
       </c>
       <c r="C8" s="9">
-        <v>5.2678880000000001</v>
+        <v>12.181229</v>
       </c>
       <c r="D8" s="9">
         <f>$C$8/C8</f>
         <v>1</v>
       </c>
       <c r="E8" s="9">
-        <f>D8/B8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="6">
         <v>2</v>
       </c>
       <c r="C9" s="7">
-        <v>3.443095</v>
+        <v>4.3996320000000004</v>
       </c>
       <c r="D9" s="5">
         <f>$C$8/C9</f>
-        <v>1.5299862478380644</v>
+        <v>2.7686926997530699</v>
       </c>
       <c r="E9" s="5">
-        <f>D9/B9</f>
-        <v>0.76499312391903218</v>
+        <f t="shared" si="0"/>
+        <v>1.3843463498765349</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="26" x14ac:dyDescent="0.3">
@@ -4305,15 +4296,15 @@
         <v>4</v>
       </c>
       <c r="C10" s="7">
-        <v>3.5855100000000002</v>
+        <v>3.0963129999999999</v>
       </c>
       <c r="D10" s="5">
         <f>$C$8/C10</f>
-        <v>1.4692158158811437</v>
+        <v>3.934107759777516</v>
       </c>
       <c r="E10" s="5">
-        <f>D10/B10</f>
-        <v>0.36730395397028592</v>
+        <f t="shared" si="0"/>
+        <v>0.98352693994437901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>